<commit_message>
added option to search directly in the source directory with xls files
</commit_message>
<xml_diff>
--- a/src/src2.xlsx
+++ b/src/src2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/imanassy/Documents/Python/excel2csv/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{440E5C5C-8943-7549-996F-51BB4565649B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{89021BC4-FA04-1349-9F51-1375CD531A0F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{FF488FF7-91CB-EB4F-9AE2-08B8F08D3F55}"/>
+    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{FF488FF7-91CB-EB4F-9AE2-08B8F08D3F55}"/>
   </bookViews>
   <sheets>
     <sheet name="tab1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Header 1</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>Igor Manassypov</t>
+  </si>
+  <si>
+    <t>Manassypov</t>
   </si>
 </sst>
 </file>
@@ -413,7 +416,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{206A8733-938B-DF47-97F1-A1D87E8E3E13}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -488,10 +491,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CA8B65E-0493-674C-B54A-167634FE38CA}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -518,6 +521,14 @@
       </c>
       <c r="B3">
         <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>